<commit_message>
change folder struct, and creation sheet line and cell values
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Turtles Sheet" sheetId="1" r:id="Re9623a4b20c54992"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rafael" sheetId="2" r:id="Rf193a719868b4496"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Turtles Sheet" sheetId="1" r:id="R8320d76f81704590"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rafael" sheetId="2" r:id="Ra097fa1565ef4625"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -16,6 +16,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1">
+      <x:c r="A1" t="str">
+        <x:v>teste</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="1">
+      <x:c r="B1" t="str">
+        <x:v>123</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>